<commit_message>
Sincronizando o repositório local baixado do Luciano com o repositório que eu criei
</commit_message>
<xml_diff>
--- a/data/input/absenteeism_data_0.xlsx
+++ b/data/input/absenteeism_data_0.xlsx
@@ -476,74 +476,74 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>93301</v>
+        <v>11789</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Lorena Souza</t>
+          <t>Marina Costa</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Atendimento ao Cliente</t>
+          <t>Vendas</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Viagem de negócios</t>
+          <t>Doença</t>
         </is>
       </c>
       <c r="E2" t="n">
         <v>2</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>45095</v>
+        <v>45081</v>
       </c>
       <c r="G2" t="n">
-        <v>7314.56</v>
+        <v>8178.01</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>25931</v>
+        <v>9953</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Evelyn Costela</t>
+          <t>Rebeca Martins</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Recursos Humanos</t>
+          <t>P&amp;D</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Consulta médica</t>
+          <t>Viagem de negócios</t>
         </is>
       </c>
       <c r="E3" t="n">
         <v>2</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>45103</v>
+        <v>45094</v>
       </c>
       <c r="G3" t="n">
-        <v>6786.2</v>
+        <v>12439.21</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>51013</v>
+        <v>78014</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>João Miguel Almeida</t>
+          <t>Lucas Gabriel da Mota</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Atendimento ao Cliente</t>
+          <t>TI</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -552,56 +552,56 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>45102</v>
+        <v>45079</v>
       </c>
       <c r="G4" t="n">
-        <v>3620.44</v>
+        <v>10532.14</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>34435</v>
+        <v>33330</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Vinicius Cunha</t>
+          <t>Luiz Miguel Pires</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>TI</t>
+          <t>Financeiro</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Problemas pessoais</t>
+          <t>Viagem de negócios</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>45106</v>
+        <v>45089</v>
       </c>
       <c r="G5" t="n">
-        <v>4888.25</v>
+        <v>7823.31</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>42301</v>
+        <v>65128</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Giovanna Sales</t>
+          <t>Ana Beatriz Dias</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Atendimento ao Cliente</t>
+          <t>Operações</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -610,114 +610,114 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>45078</v>
+        <v>45097</v>
       </c>
       <c r="G6" t="n">
-        <v>5282.73</v>
+        <v>6621.36</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>61630</v>
+        <v>25489</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>João Freitas</t>
+          <t>Nicole Caldeira</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Engenharia</t>
+          <t>Recursos Humanos</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Consulta médica</t>
+          <t>Problemas pessoais</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>45083</v>
+        <v>45089</v>
       </c>
       <c r="G7" t="n">
-        <v>6697.51</v>
+        <v>5861.1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>15497</v>
+        <v>17009</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Daniel Pires</t>
+          <t>Heitor Vieira</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Marketing</t>
+          <t>Recursos Humanos</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Viagem de negócios</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>45102</v>
+        <v>45087</v>
       </c>
       <c r="G8" t="n">
-        <v>8640.23</v>
+        <v>5645.18</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>65745</v>
+        <v>67378</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>André Cardoso</t>
+          <t>Pietro Alves</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>TI</t>
+          <t>Marketing</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Outros</t>
+          <t>Consulta médica</t>
         </is>
       </c>
       <c r="E9" t="n">
         <v>1</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>45102</v>
+        <v>45100</v>
       </c>
       <c r="G9" t="n">
-        <v>12090.83</v>
+        <v>3782.74</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>84682</v>
+        <v>1466</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Maria Vitória Freitas</t>
+          <t>Maitê Silva</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Engenharia</t>
+          <t>Atendimento ao Cliente</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -726,42 +726,42 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>45103</v>
+        <v>45105</v>
       </c>
       <c r="G10" t="n">
-        <v>4017.89</v>
+        <v>7031.39</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>69939</v>
+        <v>8824</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Mariane Martins</t>
+          <t>Fernanda Pinto</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>TI</t>
+          <t>Recursos Humanos</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Problemas pessoais</t>
+          <t>Viagem de negócios</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>45097</v>
+        <v>45104</v>
       </c>
       <c r="G11" t="n">
-        <v>4373.85</v>
+        <v>11673.54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>